<commit_message>
Generación de calidad de P1356
</commit_message>
<xml_diff>
--- a/Proyectos/2015/12/P1356 -CFDI+, Mario Govea _MO/Calidad/Checklist_Calidad_151211.xlsx
+++ b/Proyectos/2015/12/P1356 -CFDI+, Mario Govea _MO/Calidad/Checklist_Calidad_151211.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" state="visible" r:id="rId2"/>
@@ -1204,7 +1204,7 @@
   </sheetPr>
   <dimension ref="1:42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -20980,11 +20980,11 @@
       </c>
       <c r="C40" s="27" t="n">
         <f aca="false">COUNTA(Funcional!C5:C7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40" s="28" t="n">
         <f aca="false">COUNTIF(Funcional!C5:C7,"x")/(COUNTIF((Funcional!C5:C7),"x")+COUNTIF((Funcional!D5:D7),"x"))</f>
-        <v>0.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22896,8 +22896,8 @@
   </sheetPr>
   <dimension ref="A2:F16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22968,10 +22968,10 @@
       <c r="B6" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34" t="s">
+      <c r="C6" s="34" t="s">
         <v>26</v>
       </c>
+      <c r="D6" s="34"/>
       <c r="E6" s="34"/>
       <c r="F6" s="35"/>
     </row>

</xml_diff>